<commit_message>
More Game play changes
</commit_message>
<xml_diff>
--- a/assets/Arcs.xlsx
+++ b/assets/Arcs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/simonholmes/Documents/GitHub/FirePanic/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FC5C2F6-B989-0046-A8BB-770484C917D5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ADBA717-DDFD-0E4C-B8C9-3278CDEC200D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="2940" windowWidth="14160" windowHeight="24300" activeTab="1" xr2:uid="{071243AF-648E-C549-A798-77CE65D73BDA}"/>
+    <workbookView minimized="1" xWindow="840" yWindow="2940" windowWidth="14160" windowHeight="24300" activeTab="1" xr2:uid="{071243AF-648E-C549-A798-77CE65D73BDA}"/>
   </bookViews>
   <sheets>
     <sheet name="Angel 1" sheetId="4" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="6">
   <si>
     <t>x</t>
   </si>
@@ -44,6 +44,9 @@
   </si>
   <si>
     <t>Min</t>
+  </si>
+  <si>
+    <t>Gap</t>
   </si>
 </sst>
 </file>
@@ -4031,1099 +4034,1357 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73E315BE-B9FC-9547-BBBF-9775B80C3129}">
-  <dimension ref="D1:H61"/>
+  <dimension ref="D1:K61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="4:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D1" t="s">
         <v>3</v>
       </c>
       <c r="G1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="J1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D2">
-        <v>400</v>
+        <v>1500</v>
       </c>
       <c r="E2">
         <f>$D$2-(D2/2)</f>
-        <v>200</v>
+        <v>750</v>
       </c>
       <c r="G2">
         <f>D2/2</f>
-        <v>200</v>
+        <v>750</v>
       </c>
       <c r="H2">
         <f>$G$2-(G2/2)</f>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="4:8" x14ac:dyDescent="0.2">
+        <v>375</v>
+      </c>
+      <c r="J2">
+        <v>1000</v>
+      </c>
+      <c r="K2">
+        <f>INT(($J$2-J2)/250) + 3</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D3">
-        <f>D2-10</f>
-        <v>390</v>
+        <f>D2-50</f>
+        <v>1450</v>
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E61" si="0">$D$2-(D3/2)</f>
-        <v>205</v>
+        <v>775</v>
       </c>
       <c r="G3">
-        <f>G2-10</f>
-        <v>190</v>
+        <f t="shared" ref="G3:G61" si="1">G2-50</f>
+        <v>700</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H61" si="1">$G$2-(G3/2)</f>
-        <v>105</v>
-      </c>
-    </row>
-    <row r="4" spans="4:8" x14ac:dyDescent="0.2">
+        <f t="shared" ref="H3:H61" si="2">$G$2-(G3/2)</f>
+        <v>400</v>
+      </c>
+      <c r="J3">
+        <f>J2-50</f>
+        <v>950</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ref="K3:K33" si="3">INT(($J$2-J3)/250) + 3</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D4">
-        <f t="shared" ref="D4:D37" si="2">D3-10</f>
-        <v>380</v>
+        <f t="shared" ref="D4:D61" si="4">D3-50</f>
+        <v>1400</v>
       </c>
       <c r="E4">
         <f t="shared" si="0"/>
-        <v>210</v>
+        <v>800</v>
       </c>
       <c r="G4">
-        <f t="shared" ref="G4:G37" si="3">G3-10</f>
-        <v>180</v>
+        <f t="shared" si="1"/>
+        <v>650</v>
       </c>
       <c r="H4">
+        <f t="shared" si="2"/>
+        <v>425</v>
+      </c>
+      <c r="J4">
+        <f t="shared" ref="J4:J33" si="5">J3-50</f>
+        <v>900</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D5">
+        <f t="shared" si="4"/>
+        <v>1350</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>825</v>
+      </c>
+      <c r="G5">
         <f t="shared" si="1"/>
-        <v>110</v>
-      </c>
-    </row>
-    <row r="5" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D5">
-        <f t="shared" si="2"/>
-        <v>370</v>
-      </c>
-      <c r="E5">
-        <f t="shared" si="0"/>
-        <v>215</v>
-      </c>
-      <c r="G5">
+        <v>600</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="2"/>
+        <v>450</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="5"/>
+        <v>850</v>
+      </c>
+      <c r="K5">
         <f t="shared" si="3"/>
-        <v>170</v>
-      </c>
-      <c r="H5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D6">
+        <f t="shared" si="4"/>
+        <v>1300</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>850</v>
+      </c>
+      <c r="G6">
         <f t="shared" si="1"/>
-        <v>115</v>
-      </c>
-    </row>
-    <row r="6" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D6">
-        <f t="shared" si="2"/>
-        <v>360</v>
-      </c>
-      <c r="E6">
-        <f t="shared" si="0"/>
-        <v>220</v>
-      </c>
-      <c r="G6">
+        <v>550</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="2"/>
+        <v>475</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="5"/>
+        <v>800</v>
+      </c>
+      <c r="K6">
         <f t="shared" si="3"/>
-        <v>160</v>
-      </c>
-      <c r="H6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D7">
+        <f t="shared" si="4"/>
+        <v>1250</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>875</v>
+      </c>
+      <c r="G7">
         <f t="shared" si="1"/>
-        <v>120</v>
-      </c>
-    </row>
-    <row r="7" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D7">
-        <f t="shared" si="2"/>
+        <v>500</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="2"/>
+        <v>500</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="5"/>
+        <v>750</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D8">
+        <f t="shared" si="4"/>
+        <v>1200</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>900</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="1"/>
+        <v>450</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="2"/>
+        <v>525</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="5"/>
+        <v>700</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D9">
+        <f t="shared" si="4"/>
+        <v>1150</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>925</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>400</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="2"/>
+        <v>550</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="5"/>
+        <v>650</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D10">
+        <f t="shared" si="4"/>
+        <v>1100</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>950</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="1"/>
         <v>350</v>
       </c>
-      <c r="E7">
-        <f t="shared" si="0"/>
-        <v>225</v>
-      </c>
-      <c r="G7">
+      <c r="H10">
+        <f t="shared" si="2"/>
+        <v>575</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="5"/>
+        <v>600</v>
+      </c>
+      <c r="K10">
         <f t="shared" si="3"/>
-        <v>150</v>
-      </c>
-      <c r="H7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D11">
+        <f t="shared" si="4"/>
+        <v>1050</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>975</v>
+      </c>
+      <c r="G11">
         <f t="shared" si="1"/>
-        <v>125</v>
-      </c>
-    </row>
-    <row r="8" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D8">
-        <f t="shared" si="2"/>
-        <v>340</v>
-      </c>
-      <c r="E8">
-        <f t="shared" si="0"/>
-        <v>230</v>
-      </c>
-      <c r="G8">
+        <v>300</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="2"/>
+        <v>600</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="5"/>
+        <v>550</v>
+      </c>
+      <c r="K11">
         <f t="shared" si="3"/>
-        <v>140</v>
-      </c>
-      <c r="H8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D12">
+        <f t="shared" si="4"/>
+        <v>1000</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="G12">
         <f t="shared" si="1"/>
-        <v>130</v>
-      </c>
-    </row>
-    <row r="9" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D9">
-        <f t="shared" si="2"/>
-        <v>330</v>
-      </c>
-      <c r="E9">
-        <f t="shared" si="0"/>
-        <v>235</v>
-      </c>
-      <c r="G9">
+        <v>250</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="2"/>
+        <v>625</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="5"/>
+        <v>500</v>
+      </c>
+      <c r="K12">
         <f t="shared" si="3"/>
-        <v>130</v>
-      </c>
-      <c r="H9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D13">
+        <f t="shared" si="4"/>
+        <v>950</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>1025</v>
+      </c>
+      <c r="G13">
         <f t="shared" si="1"/>
-        <v>135</v>
-      </c>
-    </row>
-    <row r="10" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D10">
-        <f t="shared" si="2"/>
-        <v>320</v>
-      </c>
-      <c r="E10">
-        <f t="shared" si="0"/>
-        <v>240</v>
-      </c>
-      <c r="G10">
+        <v>200</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="2"/>
+        <v>650</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="5"/>
+        <v>450</v>
+      </c>
+      <c r="K13">
         <f t="shared" si="3"/>
-        <v>120</v>
-      </c>
-      <c r="H10">
-        <f t="shared" si="1"/>
-        <v>140</v>
-      </c>
-    </row>
-    <row r="11" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D11">
-        <f t="shared" si="2"/>
-        <v>310</v>
-      </c>
-      <c r="E11">
-        <f t="shared" si="0"/>
-        <v>245</v>
-      </c>
-      <c r="G11">
-        <f t="shared" si="3"/>
-        <v>110</v>
-      </c>
-      <c r="H11">
-        <f t="shared" si="1"/>
-        <v>145</v>
-      </c>
-    </row>
-    <row r="12" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D12">
-        <f t="shared" si="2"/>
-        <v>300</v>
-      </c>
-      <c r="E12">
-        <f t="shared" si="0"/>
-        <v>250</v>
-      </c>
-      <c r="G12">
-        <f t="shared" si="3"/>
-        <v>100</v>
-      </c>
-      <c r="H12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D14">
+        <f t="shared" si="4"/>
+        <v>900</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>1050</v>
+      </c>
+      <c r="G14">
         <f t="shared" si="1"/>
         <v>150</v>
       </c>
-    </row>
-    <row r="13" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D13">
-        <f t="shared" si="2"/>
-        <v>290</v>
-      </c>
-      <c r="E13">
-        <f t="shared" si="0"/>
-        <v>255</v>
-      </c>
-      <c r="G13">
+      <c r="H14">
+        <f t="shared" si="2"/>
+        <v>675</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="5"/>
+        <v>400</v>
+      </c>
+      <c r="K14">
         <f t="shared" si="3"/>
-        <v>90</v>
-      </c>
-      <c r="H13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D15">
+        <f t="shared" si="4"/>
+        <v>850</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>1075</v>
+      </c>
+      <c r="G15">
         <f t="shared" si="1"/>
-        <v>155</v>
-      </c>
-    </row>
-    <row r="14" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D14">
-        <f t="shared" si="2"/>
-        <v>280</v>
-      </c>
-      <c r="E14">
-        <f t="shared" si="0"/>
-        <v>260</v>
-      </c>
-      <c r="G14">
+        <v>100</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="2"/>
+        <v>700</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="5"/>
+        <v>350</v>
+      </c>
+      <c r="K15">
         <f t="shared" si="3"/>
-        <v>80</v>
-      </c>
-      <c r="H14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D16">
+        <f t="shared" si="4"/>
+        <v>800</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>1100</v>
+      </c>
+      <c r="G16">
         <f t="shared" si="1"/>
-        <v>160</v>
-      </c>
-    </row>
-    <row r="15" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D15">
-        <f t="shared" si="2"/>
-        <v>270</v>
-      </c>
-      <c r="E15">
-        <f t="shared" si="0"/>
-        <v>265</v>
-      </c>
-      <c r="G15">
+        <v>50</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="2"/>
+        <v>725</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="5"/>
+        <v>300</v>
+      </c>
+      <c r="K16">
         <f t="shared" si="3"/>
-        <v>70</v>
-      </c>
-      <c r="H15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D17">
+        <f t="shared" si="4"/>
+        <v>750</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>1125</v>
+      </c>
+      <c r="G17">
         <f t="shared" si="1"/>
-        <v>165</v>
-      </c>
-    </row>
-    <row r="16" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D16">
-        <f t="shared" si="2"/>
-        <v>260</v>
-      </c>
-      <c r="E16">
-        <f t="shared" si="0"/>
-        <v>270</v>
-      </c>
-      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="2"/>
+        <v>750</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="5"/>
+        <v>250</v>
+      </c>
+      <c r="K17">
         <f t="shared" si="3"/>
-        <v>60</v>
-      </c>
-      <c r="H16">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D18">
+        <f t="shared" si="4"/>
+        <v>700</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>1150</v>
+      </c>
+      <c r="G18">
         <f t="shared" si="1"/>
-        <v>170</v>
-      </c>
-    </row>
-    <row r="17" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D17">
-        <f t="shared" si="2"/>
-        <v>250</v>
-      </c>
-      <c r="E17">
-        <f t="shared" si="0"/>
-        <v>275</v>
-      </c>
-      <c r="G17">
+        <v>-50</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="2"/>
+        <v>775</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="5"/>
+        <v>200</v>
+      </c>
+      <c r="K18">
         <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D19">
+        <f t="shared" si="4"/>
+        <v>650</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>1175</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="1"/>
+        <v>-100</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="2"/>
+        <v>800</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="5"/>
+        <v>150</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D20">
+        <f t="shared" si="4"/>
+        <v>600</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>1200</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="1"/>
+        <v>-150</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="2"/>
+        <v>825</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="5"/>
+        <v>100</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D21">
+        <f t="shared" si="4"/>
+        <v>550</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="0"/>
+        <v>1225</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="1"/>
+        <v>-200</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="2"/>
+        <v>850</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="5"/>
         <v>50</v>
       </c>
-      <c r="H17">
+      <c r="K21">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D22">
+        <f t="shared" si="4"/>
+        <v>500</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="0"/>
+        <v>1250</v>
+      </c>
+      <c r="G22">
         <f t="shared" si="1"/>
-        <v>175</v>
-      </c>
-    </row>
-    <row r="18" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D18">
-        <f t="shared" si="2"/>
-        <v>240</v>
-      </c>
-      <c r="E18">
-        <f t="shared" si="0"/>
-        <v>280</v>
-      </c>
-      <c r="G18">
+        <v>-250</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="2"/>
+        <v>875</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K22">
         <f t="shared" si="3"/>
-        <v>40</v>
-      </c>
-      <c r="H18">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D23">
+        <f t="shared" si="4"/>
+        <v>450</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="0"/>
+        <v>1275</v>
+      </c>
+      <c r="G23">
         <f t="shared" si="1"/>
-        <v>180</v>
-      </c>
-    </row>
-    <row r="19" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D19">
-        <f t="shared" si="2"/>
-        <v>230</v>
-      </c>
-      <c r="E19">
-        <f t="shared" si="0"/>
-        <v>285</v>
-      </c>
-      <c r="G19">
+        <v>-300</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="2"/>
+        <v>900</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="5"/>
+        <v>-50</v>
+      </c>
+      <c r="K23">
         <f t="shared" si="3"/>
-        <v>30</v>
-      </c>
-      <c r="H19">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D24">
+        <f t="shared" si="4"/>
+        <v>400</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="0"/>
+        <v>1300</v>
+      </c>
+      <c r="G24">
         <f t="shared" si="1"/>
-        <v>185</v>
-      </c>
-    </row>
-    <row r="20" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D20">
-        <f t="shared" si="2"/>
-        <v>220</v>
-      </c>
-      <c r="E20">
-        <f t="shared" si="0"/>
-        <v>290</v>
-      </c>
-      <c r="G20">
+        <v>-350</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="2"/>
+        <v>925</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="5"/>
+        <v>-100</v>
+      </c>
+      <c r="K24">
         <f t="shared" si="3"/>
-        <v>20</v>
-      </c>
-      <c r="H20">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D25">
+        <f t="shared" si="4"/>
+        <v>350</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="0"/>
+        <v>1325</v>
+      </c>
+      <c r="G25">
         <f t="shared" si="1"/>
-        <v>190</v>
-      </c>
-    </row>
-    <row r="21" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D21">
-        <f t="shared" si="2"/>
-        <v>210</v>
-      </c>
-      <c r="E21">
-        <f t="shared" si="0"/>
-        <v>295</v>
-      </c>
-      <c r="G21">
+        <v>-400</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="2"/>
+        <v>950</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="5"/>
+        <v>-150</v>
+      </c>
+      <c r="K25">
         <f t="shared" si="3"/>
-        <v>10</v>
-      </c>
-      <c r="H21">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D26">
+        <f t="shared" si="4"/>
+        <v>300</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="0"/>
+        <v>1350</v>
+      </c>
+      <c r="G26">
         <f t="shared" si="1"/>
-        <v>195</v>
-      </c>
-    </row>
-    <row r="22" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D22">
-        <f t="shared" si="2"/>
-        <v>200</v>
-      </c>
-      <c r="E22">
-        <f t="shared" si="0"/>
-        <v>300</v>
-      </c>
-      <c r="G22">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="H22">
-        <f t="shared" si="1"/>
-        <v>200</v>
-      </c>
-    </row>
-    <row r="23" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D23">
-        <f t="shared" si="2"/>
-        <v>190</v>
-      </c>
-      <c r="E23">
-        <f t="shared" si="0"/>
-        <v>305</v>
-      </c>
-      <c r="G23">
-        <f t="shared" si="3"/>
-        <v>-10</v>
-      </c>
-      <c r="H23">
-        <f t="shared" si="1"/>
-        <v>205</v>
-      </c>
-    </row>
-    <row r="24" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D24">
-        <f t="shared" si="2"/>
-        <v>180</v>
-      </c>
-      <c r="E24">
-        <f t="shared" si="0"/>
-        <v>310</v>
-      </c>
-      <c r="G24">
-        <f t="shared" si="3"/>
-        <v>-20</v>
-      </c>
-      <c r="H24">
-        <f t="shared" si="1"/>
-        <v>210</v>
-      </c>
-    </row>
-    <row r="25" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D25">
-        <f t="shared" si="2"/>
-        <v>170</v>
-      </c>
-      <c r="E25">
-        <f t="shared" si="0"/>
-        <v>315</v>
-      </c>
-      <c r="G25">
-        <f t="shared" si="3"/>
-        <v>-30</v>
-      </c>
-      <c r="H25">
-        <f t="shared" si="1"/>
-        <v>215</v>
-      </c>
-    </row>
-    <row r="26" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D26">
-        <f t="shared" si="2"/>
-        <v>160</v>
-      </c>
-      <c r="E26">
-        <f t="shared" si="0"/>
-        <v>320</v>
-      </c>
-      <c r="G26">
-        <f t="shared" si="3"/>
-        <v>-40</v>
+        <v>-450</v>
       </c>
       <c r="H26">
-        <f t="shared" si="1"/>
-        <v>220</v>
-      </c>
-    </row>
-    <row r="27" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D27">
-        <f t="shared" si="2"/>
-        <v>150</v>
-      </c>
-      <c r="E27">
-        <f t="shared" si="0"/>
-        <v>325</v>
-      </c>
-      <c r="G27">
-        <f t="shared" si="3"/>
-        <v>-50</v>
-      </c>
-      <c r="H27">
-        <f t="shared" si="1"/>
-        <v>225</v>
-      </c>
-    </row>
-    <row r="28" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D28">
-        <f t="shared" si="2"/>
-        <v>140</v>
-      </c>
-      <c r="E28">
-        <f t="shared" si="0"/>
-        <v>330</v>
-      </c>
-      <c r="G28">
-        <f t="shared" si="3"/>
-        <v>-60</v>
-      </c>
-      <c r="H28">
-        <f t="shared" si="1"/>
-        <v>230</v>
-      </c>
-    </row>
-    <row r="29" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D29">
-        <f t="shared" si="2"/>
-        <v>130</v>
-      </c>
-      <c r="E29">
-        <f t="shared" si="0"/>
-        <v>335</v>
-      </c>
-      <c r="G29">
-        <f t="shared" si="3"/>
-        <v>-70</v>
-      </c>
-      <c r="H29">
-        <f t="shared" si="1"/>
-        <v>235</v>
-      </c>
-    </row>
-    <row r="30" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D30">
-        <f t="shared" si="2"/>
-        <v>120</v>
-      </c>
-      <c r="E30">
-        <f t="shared" si="0"/>
-        <v>340</v>
-      </c>
-      <c r="G30">
-        <f t="shared" si="3"/>
-        <v>-80</v>
-      </c>
-      <c r="H30">
-        <f t="shared" si="1"/>
-        <v>240</v>
-      </c>
-    </row>
-    <row r="31" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D31">
-        <f t="shared" si="2"/>
-        <v>110</v>
-      </c>
-      <c r="E31">
-        <f t="shared" si="0"/>
-        <v>345</v>
-      </c>
-      <c r="G31">
-        <f t="shared" si="3"/>
-        <v>-90</v>
-      </c>
-      <c r="H31">
-        <f t="shared" si="1"/>
-        <v>245</v>
-      </c>
-    </row>
-    <row r="32" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D32">
-        <f t="shared" si="2"/>
-        <v>100</v>
-      </c>
-      <c r="E32">
-        <f t="shared" si="0"/>
-        <v>350</v>
-      </c>
-      <c r="G32">
-        <f t="shared" si="3"/>
-        <v>-100</v>
-      </c>
-      <c r="H32">
-        <f t="shared" si="1"/>
-        <v>250</v>
-      </c>
-    </row>
-    <row r="33" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D33">
-        <f t="shared" si="2"/>
-        <v>90</v>
-      </c>
-      <c r="E33">
-        <f t="shared" si="0"/>
-        <v>355</v>
-      </c>
-      <c r="G33">
-        <f t="shared" si="3"/>
-        <v>-110</v>
-      </c>
-      <c r="H33">
-        <f t="shared" si="1"/>
-        <v>255</v>
-      </c>
-    </row>
-    <row r="34" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D34">
-        <f t="shared" si="2"/>
-        <v>80</v>
-      </c>
-      <c r="E34">
-        <f t="shared" si="0"/>
-        <v>360</v>
-      </c>
-      <c r="G34">
-        <f t="shared" si="3"/>
-        <v>-120</v>
-      </c>
-      <c r="H34">
-        <f t="shared" si="1"/>
-        <v>260</v>
-      </c>
-    </row>
-    <row r="35" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D35">
-        <f t="shared" si="2"/>
-        <v>70</v>
-      </c>
-      <c r="E35">
-        <f t="shared" si="0"/>
-        <v>365</v>
-      </c>
-      <c r="G35">
-        <f t="shared" si="3"/>
-        <v>-130</v>
-      </c>
-      <c r="H35">
-        <f t="shared" si="1"/>
-        <v>265</v>
-      </c>
-    </row>
-    <row r="36" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D36">
-        <f t="shared" si="2"/>
-        <v>60</v>
-      </c>
-      <c r="E36">
-        <f t="shared" si="0"/>
-        <v>370</v>
-      </c>
-      <c r="G36">
-        <f t="shared" si="3"/>
-        <v>-140</v>
-      </c>
-      <c r="H36">
-        <f t="shared" si="1"/>
-        <v>270</v>
-      </c>
-    </row>
-    <row r="37" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D37">
-        <f t="shared" si="2"/>
-        <v>50</v>
-      </c>
-      <c r="E37">
-        <f t="shared" si="0"/>
-        <v>375</v>
-      </c>
-      <c r="G37">
-        <f t="shared" si="3"/>
-        <v>-150</v>
-      </c>
-      <c r="H37">
-        <f t="shared" si="1"/>
-        <v>275</v>
-      </c>
-    </row>
-    <row r="38" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D38">
-        <f t="shared" ref="D38:D61" si="4">D37-10</f>
-        <v>40</v>
-      </c>
-      <c r="E38">
-        <f t="shared" si="0"/>
-        <v>380</v>
-      </c>
-      <c r="G38">
-        <f t="shared" ref="G38:G61" si="5">G37-10</f>
-        <v>-160</v>
-      </c>
-      <c r="H38">
-        <f t="shared" si="1"/>
-        <v>280</v>
-      </c>
-    </row>
-    <row r="39" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D39">
-        <f t="shared" si="4"/>
-        <v>30</v>
-      </c>
-      <c r="E39">
-        <f t="shared" si="0"/>
-        <v>385</v>
-      </c>
-      <c r="G39">
-        <f t="shared" si="5"/>
-        <v>-170</v>
-      </c>
-      <c r="H39">
-        <f t="shared" si="1"/>
-        <v>285</v>
-      </c>
-    </row>
-    <row r="40" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D40">
-        <f t="shared" si="4"/>
-        <v>20</v>
-      </c>
-      <c r="E40">
-        <f t="shared" si="0"/>
-        <v>390</v>
-      </c>
-      <c r="G40">
-        <f t="shared" si="5"/>
-        <v>-180</v>
-      </c>
-      <c r="H40">
-        <f t="shared" si="1"/>
-        <v>290</v>
-      </c>
-    </row>
-    <row r="41" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D41">
-        <f t="shared" si="4"/>
-        <v>10</v>
-      </c>
-      <c r="E41">
-        <f t="shared" si="0"/>
-        <v>395</v>
-      </c>
-      <c r="G41">
-        <f t="shared" si="5"/>
-        <v>-190</v>
-      </c>
-      <c r="H41">
-        <f t="shared" si="1"/>
-        <v>295</v>
-      </c>
-    </row>
-    <row r="42" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D42">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="E42">
-        <f t="shared" si="0"/>
-        <v>400</v>
-      </c>
-      <c r="G42">
+        <f t="shared" si="2"/>
+        <v>975</v>
+      </c>
+      <c r="J26">
         <f t="shared" si="5"/>
         <v>-200</v>
       </c>
-      <c r="H42">
+      <c r="K26">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D27">
+        <f t="shared" si="4"/>
+        <v>250</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="0"/>
+        <v>1375</v>
+      </c>
+      <c r="G27">
         <f t="shared" si="1"/>
-        <v>300</v>
-      </c>
-    </row>
-    <row r="43" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D43">
-        <f t="shared" si="4"/>
-        <v>-10</v>
-      </c>
-      <c r="E43">
-        <f t="shared" si="0"/>
-        <v>405</v>
-      </c>
-      <c r="G43">
-        <f t="shared" si="5"/>
-        <v>-210</v>
-      </c>
-      <c r="H43">
-        <f t="shared" si="1"/>
-        <v>305</v>
-      </c>
-    </row>
-    <row r="44" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D44">
-        <f t="shared" si="4"/>
-        <v>-20</v>
-      </c>
-      <c r="E44">
-        <f t="shared" si="0"/>
-        <v>410</v>
-      </c>
-      <c r="G44">
-        <f t="shared" si="5"/>
-        <v>-220</v>
-      </c>
-      <c r="H44">
-        <f t="shared" si="1"/>
-        <v>310</v>
-      </c>
-    </row>
-    <row r="45" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D45">
-        <f t="shared" si="4"/>
-        <v>-30</v>
-      </c>
-      <c r="E45">
-        <f t="shared" si="0"/>
-        <v>415</v>
-      </c>
-      <c r="G45">
-        <f t="shared" si="5"/>
-        <v>-230</v>
-      </c>
-      <c r="H45">
-        <f t="shared" si="1"/>
-        <v>315</v>
-      </c>
-    </row>
-    <row r="46" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D46">
-        <f t="shared" si="4"/>
-        <v>-40</v>
-      </c>
-      <c r="E46">
-        <f t="shared" si="0"/>
-        <v>420</v>
-      </c>
-      <c r="G46">
-        <f t="shared" si="5"/>
-        <v>-240</v>
-      </c>
-      <c r="H46">
-        <f t="shared" si="1"/>
-        <v>320</v>
-      </c>
-    </row>
-    <row r="47" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D47">
-        <f t="shared" si="4"/>
-        <v>-50</v>
-      </c>
-      <c r="E47">
-        <f t="shared" si="0"/>
-        <v>425</v>
-      </c>
-      <c r="G47">
+        <v>-500</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="2"/>
+        <v>1000</v>
+      </c>
+      <c r="J27">
         <f t="shared" si="5"/>
         <v>-250</v>
       </c>
+      <c r="K27">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D28">
+        <f t="shared" si="4"/>
+        <v>200</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="0"/>
+        <v>1400</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="1"/>
+        <v>-550</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="2"/>
+        <v>1025</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="5"/>
+        <v>-300</v>
+      </c>
+      <c r="K28">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D29">
+        <f t="shared" si="4"/>
+        <v>150</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="0"/>
+        <v>1425</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="1"/>
+        <v>-600</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="2"/>
+        <v>1050</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="5"/>
+        <v>-350</v>
+      </c>
+      <c r="K29">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D30">
+        <f t="shared" si="4"/>
+        <v>100</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="0"/>
+        <v>1450</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="1"/>
+        <v>-650</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="2"/>
+        <v>1075</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="5"/>
+        <v>-400</v>
+      </c>
+      <c r="K30">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D31">
+        <f t="shared" si="4"/>
+        <v>50</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="0"/>
+        <v>1475</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="1"/>
+        <v>-700</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="2"/>
+        <v>1100</v>
+      </c>
+      <c r="J31">
+        <f t="shared" si="5"/>
+        <v>-450</v>
+      </c>
+      <c r="K31">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D32">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="0"/>
+        <v>1500</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="1"/>
+        <v>-750</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="2"/>
+        <v>1125</v>
+      </c>
+      <c r="J32">
+        <f t="shared" si="5"/>
+        <v>-500</v>
+      </c>
+      <c r="K32">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D33">
+        <f t="shared" si="4"/>
+        <v>-50</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="0"/>
+        <v>1525</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="1"/>
+        <v>-800</v>
+      </c>
+      <c r="H33">
+        <f t="shared" si="2"/>
+        <v>1150</v>
+      </c>
+      <c r="J33">
+        <f t="shared" si="5"/>
+        <v>-550</v>
+      </c>
+      <c r="K33">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D34">
+        <f t="shared" si="4"/>
+        <v>-100</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="0"/>
+        <v>1550</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="1"/>
+        <v>-850</v>
+      </c>
+      <c r="H34">
+        <f t="shared" si="2"/>
+        <v>1175</v>
+      </c>
+    </row>
+    <row r="35" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D35">
+        <f t="shared" si="4"/>
+        <v>-150</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="0"/>
+        <v>1575</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="1"/>
+        <v>-900</v>
+      </c>
+      <c r="H35">
+        <f t="shared" si="2"/>
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="36" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D36">
+        <f t="shared" si="4"/>
+        <v>-200</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="0"/>
+        <v>1600</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="1"/>
+        <v>-950</v>
+      </c>
+      <c r="H36">
+        <f t="shared" si="2"/>
+        <v>1225</v>
+      </c>
+    </row>
+    <row r="37" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D37">
+        <f t="shared" si="4"/>
+        <v>-250</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="0"/>
+        <v>1625</v>
+      </c>
+      <c r="G37">
+        <f t="shared" si="1"/>
+        <v>-1000</v>
+      </c>
+      <c r="H37">
+        <f t="shared" si="2"/>
+        <v>1250</v>
+      </c>
+    </row>
+    <row r="38" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D38">
+        <f t="shared" si="4"/>
+        <v>-300</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="0"/>
+        <v>1650</v>
+      </c>
+      <c r="G38">
+        <f t="shared" si="1"/>
+        <v>-1050</v>
+      </c>
+      <c r="H38">
+        <f t="shared" si="2"/>
+        <v>1275</v>
+      </c>
+    </row>
+    <row r="39" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D39">
+        <f t="shared" si="4"/>
+        <v>-350</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="0"/>
+        <v>1675</v>
+      </c>
+      <c r="G39">
+        <f t="shared" si="1"/>
+        <v>-1100</v>
+      </c>
+      <c r="H39">
+        <f t="shared" si="2"/>
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="40" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D40">
+        <f t="shared" si="4"/>
+        <v>-400</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="0"/>
+        <v>1700</v>
+      </c>
+      <c r="G40">
+        <f t="shared" si="1"/>
+        <v>-1150</v>
+      </c>
+      <c r="H40">
+        <f t="shared" si="2"/>
+        <v>1325</v>
+      </c>
+    </row>
+    <row r="41" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D41">
+        <f t="shared" si="4"/>
+        <v>-450</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="0"/>
+        <v>1725</v>
+      </c>
+      <c r="G41">
+        <f t="shared" si="1"/>
+        <v>-1200</v>
+      </c>
+      <c r="H41">
+        <f t="shared" si="2"/>
+        <v>1350</v>
+      </c>
+    </row>
+    <row r="42" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D42">
+        <f t="shared" si="4"/>
+        <v>-500</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="0"/>
+        <v>1750</v>
+      </c>
+      <c r="G42">
+        <f t="shared" si="1"/>
+        <v>-1250</v>
+      </c>
+      <c r="H42">
+        <f t="shared" si="2"/>
+        <v>1375</v>
+      </c>
+    </row>
+    <row r="43" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D43">
+        <f t="shared" si="4"/>
+        <v>-550</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="0"/>
+        <v>1775</v>
+      </c>
+      <c r="G43">
+        <f t="shared" si="1"/>
+        <v>-1300</v>
+      </c>
+      <c r="H43">
+        <f t="shared" si="2"/>
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="44" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D44">
+        <f t="shared" si="4"/>
+        <v>-600</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="0"/>
+        <v>1800</v>
+      </c>
+      <c r="G44">
+        <f t="shared" si="1"/>
+        <v>-1350</v>
+      </c>
+      <c r="H44">
+        <f t="shared" si="2"/>
+        <v>1425</v>
+      </c>
+    </row>
+    <row r="45" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D45">
+        <f t="shared" si="4"/>
+        <v>-650</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="0"/>
+        <v>1825</v>
+      </c>
+      <c r="G45">
+        <f t="shared" si="1"/>
+        <v>-1400</v>
+      </c>
+      <c r="H45">
+        <f t="shared" si="2"/>
+        <v>1450</v>
+      </c>
+    </row>
+    <row r="46" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D46">
+        <f t="shared" si="4"/>
+        <v>-700</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="0"/>
+        <v>1850</v>
+      </c>
+      <c r="G46">
+        <f t="shared" si="1"/>
+        <v>-1450</v>
+      </c>
+      <c r="H46">
+        <f t="shared" si="2"/>
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="47" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D47">
+        <f t="shared" si="4"/>
+        <v>-750</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="0"/>
+        <v>1875</v>
+      </c>
+      <c r="G47">
+        <f t="shared" si="1"/>
+        <v>-1500</v>
+      </c>
       <c r="H47">
+        <f t="shared" si="2"/>
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="48" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D48">
+        <f t="shared" si="4"/>
+        <v>-800</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="0"/>
+        <v>1900</v>
+      </c>
+      <c r="G48">
         <f t="shared" si="1"/>
-        <v>325</v>
-      </c>
-    </row>
-    <row r="48" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D48">
-        <f t="shared" si="4"/>
-        <v>-60</v>
-      </c>
-      <c r="E48">
-        <f t="shared" si="0"/>
-        <v>430</v>
-      </c>
-      <c r="G48">
-        <f t="shared" si="5"/>
-        <v>-260</v>
+        <v>-1550</v>
       </c>
       <c r="H48">
-        <f t="shared" si="1"/>
-        <v>330</v>
+        <f t="shared" si="2"/>
+        <v>1525</v>
       </c>
     </row>
     <row r="49" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D49">
         <f t="shared" si="4"/>
-        <v>-70</v>
+        <v>-850</v>
       </c>
       <c r="E49">
         <f t="shared" si="0"/>
-        <v>435</v>
+        <v>1925</v>
       </c>
       <c r="G49">
-        <f t="shared" si="5"/>
-        <v>-270</v>
+        <f t="shared" si="1"/>
+        <v>-1600</v>
       </c>
       <c r="H49">
-        <f t="shared" si="1"/>
-        <v>335</v>
+        <f t="shared" si="2"/>
+        <v>1550</v>
       </c>
     </row>
     <row r="50" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D50">
         <f t="shared" si="4"/>
-        <v>-80</v>
+        <v>-900</v>
       </c>
       <c r="E50">
         <f t="shared" si="0"/>
-        <v>440</v>
+        <v>1950</v>
       </c>
       <c r="G50">
-        <f t="shared" si="5"/>
-        <v>-280</v>
+        <f t="shared" si="1"/>
+        <v>-1650</v>
       </c>
       <c r="H50">
-        <f t="shared" si="1"/>
-        <v>340</v>
+        <f t="shared" si="2"/>
+        <v>1575</v>
       </c>
     </row>
     <row r="51" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D51">
         <f t="shared" si="4"/>
-        <v>-90</v>
+        <v>-950</v>
       </c>
       <c r="E51">
         <f t="shared" si="0"/>
-        <v>445</v>
+        <v>1975</v>
       </c>
       <c r="G51">
-        <f t="shared" si="5"/>
-        <v>-290</v>
+        <f t="shared" si="1"/>
+        <v>-1700</v>
       </c>
       <c r="H51">
-        <f t="shared" si="1"/>
-        <v>345</v>
+        <f t="shared" si="2"/>
+        <v>1600</v>
       </c>
     </row>
     <row r="52" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D52">
         <f t="shared" si="4"/>
-        <v>-100</v>
+        <v>-1000</v>
       </c>
       <c r="E52">
         <f t="shared" si="0"/>
-        <v>450</v>
+        <v>2000</v>
       </c>
       <c r="G52">
-        <f t="shared" si="5"/>
-        <v>-300</v>
+        <f t="shared" si="1"/>
+        <v>-1750</v>
       </c>
       <c r="H52">
-        <f t="shared" si="1"/>
-        <v>350</v>
+        <f t="shared" si="2"/>
+        <v>1625</v>
       </c>
     </row>
     <row r="53" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D53">
         <f t="shared" si="4"/>
-        <v>-110</v>
+        <v>-1050</v>
       </c>
       <c r="E53">
         <f t="shared" si="0"/>
-        <v>455</v>
+        <v>2025</v>
       </c>
       <c r="G53">
-        <f t="shared" si="5"/>
-        <v>-310</v>
+        <f t="shared" si="1"/>
+        <v>-1800</v>
       </c>
       <c r="H53">
-        <f t="shared" si="1"/>
-        <v>355</v>
+        <f t="shared" si="2"/>
+        <v>1650</v>
       </c>
     </row>
     <row r="54" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D54">
         <f t="shared" si="4"/>
-        <v>-120</v>
+        <v>-1100</v>
       </c>
       <c r="E54">
         <f t="shared" si="0"/>
-        <v>460</v>
+        <v>2050</v>
       </c>
       <c r="G54">
-        <f t="shared" si="5"/>
-        <v>-320</v>
+        <f t="shared" si="1"/>
+        <v>-1850</v>
       </c>
       <c r="H54">
-        <f t="shared" si="1"/>
-        <v>360</v>
+        <f t="shared" si="2"/>
+        <v>1675</v>
       </c>
     </row>
     <row r="55" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D55">
         <f t="shared" si="4"/>
-        <v>-130</v>
+        <v>-1150</v>
       </c>
       <c r="E55">
         <f t="shared" si="0"/>
-        <v>465</v>
+        <v>2075</v>
       </c>
       <c r="G55">
-        <f t="shared" si="5"/>
-        <v>-330</v>
+        <f t="shared" si="1"/>
+        <v>-1900</v>
       </c>
       <c r="H55">
-        <f t="shared" si="1"/>
-        <v>365</v>
+        <f t="shared" si="2"/>
+        <v>1700</v>
       </c>
     </row>
     <row r="56" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D56">
         <f t="shared" si="4"/>
-        <v>-140</v>
+        <v>-1200</v>
       </c>
       <c r="E56">
         <f t="shared" si="0"/>
-        <v>470</v>
+        <v>2100</v>
       </c>
       <c r="G56">
-        <f t="shared" si="5"/>
-        <v>-340</v>
+        <f t="shared" si="1"/>
+        <v>-1950</v>
       </c>
       <c r="H56">
-        <f t="shared" si="1"/>
-        <v>370</v>
+        <f t="shared" si="2"/>
+        <v>1725</v>
       </c>
     </row>
     <row r="57" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D57">
         <f t="shared" si="4"/>
-        <v>-150</v>
+        <v>-1250</v>
       </c>
       <c r="E57">
         <f t="shared" si="0"/>
-        <v>475</v>
+        <v>2125</v>
       </c>
       <c r="G57">
-        <f t="shared" si="5"/>
-        <v>-350</v>
+        <f t="shared" si="1"/>
+        <v>-2000</v>
       </c>
       <c r="H57">
-        <f t="shared" si="1"/>
-        <v>375</v>
+        <f t="shared" si="2"/>
+        <v>1750</v>
       </c>
     </row>
     <row r="58" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D58">
         <f t="shared" si="4"/>
-        <v>-160</v>
+        <v>-1300</v>
       </c>
       <c r="E58">
         <f t="shared" si="0"/>
-        <v>480</v>
+        <v>2150</v>
       </c>
       <c r="G58">
-        <f t="shared" si="5"/>
-        <v>-360</v>
+        <f t="shared" si="1"/>
+        <v>-2050</v>
       </c>
       <c r="H58">
-        <f t="shared" si="1"/>
-        <v>380</v>
+        <f t="shared" si="2"/>
+        <v>1775</v>
       </c>
     </row>
     <row r="59" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D59">
         <f t="shared" si="4"/>
-        <v>-170</v>
+        <v>-1350</v>
       </c>
       <c r="E59">
         <f t="shared" si="0"/>
-        <v>485</v>
+        <v>2175</v>
       </c>
       <c r="G59">
-        <f t="shared" si="5"/>
-        <v>-370</v>
+        <f t="shared" si="1"/>
+        <v>-2100</v>
       </c>
       <c r="H59">
-        <f t="shared" si="1"/>
-        <v>385</v>
+        <f t="shared" si="2"/>
+        <v>1800</v>
       </c>
     </row>
     <row r="60" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D60">
         <f t="shared" si="4"/>
-        <v>-180</v>
+        <v>-1400</v>
       </c>
       <c r="E60">
         <f t="shared" si="0"/>
-        <v>490</v>
+        <v>2200</v>
       </c>
       <c r="G60">
-        <f t="shared" si="5"/>
-        <v>-380</v>
+        <f t="shared" si="1"/>
+        <v>-2150</v>
       </c>
       <c r="H60">
-        <f t="shared" si="1"/>
-        <v>390</v>
+        <f t="shared" si="2"/>
+        <v>1825</v>
       </c>
     </row>
     <row r="61" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D61">
         <f t="shared" si="4"/>
-        <v>-190</v>
+        <v>-1450</v>
       </c>
       <c r="E61">
         <f t="shared" si="0"/>
-        <v>495</v>
+        <v>2225</v>
       </c>
       <c r="G61">
-        <f t="shared" si="5"/>
-        <v>-390</v>
+        <f t="shared" si="1"/>
+        <v>-2200</v>
       </c>
       <c r="H61">
-        <f t="shared" si="1"/>
-        <v>395</v>
+        <f t="shared" si="2"/>
+        <v>1850</v>
       </c>
     </row>
   </sheetData>

</xml_diff>